<commit_message>
Mise à jour trace
</commit_message>
<xml_diff>
--- a/Journal des difficultés et solutions mises en oeuvre_Stage 4A_GPSE_24-25.xlsx
+++ b/Journal des difficultés et solutions mises en oeuvre_Stage 4A_GPSE_24-25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dacruzc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mslfso\services$\Moytests\02_Activité Service Standard Test\STAGES &amp; APPRENTIS\CEDRIC DA CRUZ\Documents Stage (Eval &amp; Compétences)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68FE168-6A85-4174-AAD3-EB841A6256F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C379552E-4542-430C-BB01-B528AAD1A41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Période 0 (avant)" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>En fonction de vos missions de stage, veuillez faire le lien avec votre référentiel de compétences</t>
   </si>
@@ -165,16 +165,46 @@
   <si>
     <t>Developper du code ou des librairies existantes</t>
   </si>
+  <si>
+    <t>- Programme de test + Interface Homme-Machine sous ATEasy
+- Création d'un prototype pour valider la solution
+- Campagne de test sur prototype pour valider prottotype + IHM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Réaliser une IHM
+- Développer du code ou des librairies
+- Programmer dans un langage informatique﻿
+- Valider un prototype</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Triple Etat de la carte en Idle (port sans branchement)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Modification du code ATEasy pour le prendre en compte</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - IHM + protocole de test sous ATEasy
+- Photo prototype  
+- Photo test avec prototype
+- Exemple de fichier de Log</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -776,89 +806,131 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -873,13 +945,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -888,115 +960,31 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1005,12 +993,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1023,8 +1056,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="8" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1490,7 +1535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15:G15"/>
     </sheetView>
   </sheetViews>
@@ -1515,260 +1560,255 @@
       <c r="N1" s="3"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="44"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="31"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="47"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="34"/>
       <c r="P4" s="25"/>
       <c r="Q4" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="47"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="34"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="27" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="47"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="47"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="34"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="50"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
     </row>
     <row r="12" spans="1:17" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="54" t="s">
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="55"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" spans="1:17" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="86" t="s">
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="40"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="54"/>
     </row>
     <row r="14" spans="1:17" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="38" t="s">
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="40"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="54"/>
     </row>
     <row r="15" spans="1:17" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="32"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="46"/>
     </row>
     <row r="16" spans="1:17" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="32"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="46"/>
     </row>
     <row r="17" spans="2:14" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="35"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B3:N8"/>
-    <mergeCell ref="B10:G11"/>
-    <mergeCell ref="H10:N11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="H12:N12"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="H16:N16"/>
     <mergeCell ref="B17:G17"/>
@@ -1779,6 +1819,11 @@
     <mergeCell ref="H14:N14"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="H15:N15"/>
+    <mergeCell ref="B3:N8"/>
+    <mergeCell ref="B10:G11"/>
+    <mergeCell ref="H10:N11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="H12:N12"/>
   </mergeCells>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1803,11 +1848,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -1838,172 +1883,165 @@
     </row>
     <row r="6" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="77" t="s">
+      <c r="G6" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="71"/>
+      <c r="H6" s="57"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="76"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="71"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="57"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="23">
         <v>45782</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="71"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="57"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="71"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="23">
         <v>45800</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="71"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="71"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="57"/>
     </row>
     <row r="12" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="71"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="57"/>
     </row>
     <row r="30" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D30" s="61" t="s">
+      <c r="D30" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="64" t="s">
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="62"/>
-      <c r="O30" s="62"/>
-      <c r="P30" s="65"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="74"/>
+      <c r="O30" s="74"/>
+      <c r="P30" s="77"/>
     </row>
     <row r="31" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D31" s="66" t="s">
+      <c r="D31" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="69" t="s">
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="K31" s="67"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="67"/>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
-      <c r="P31" s="70"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="79"/>
+      <c r="P31" s="82"/>
     </row>
     <row r="32" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D32" s="56" t="s">
+      <c r="D32" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="59" t="s">
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="57"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="57"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="60"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="72"/>
     </row>
     <row r="33" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="59" t="s">
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="K33" s="57"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="57"/>
-      <c r="P33" s="60"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="H6:H12"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="C6:C12"/>
-    <mergeCell ref="D6:D12"/>
-    <mergeCell ref="E6:E12"/>
-    <mergeCell ref="F6:F12"/>
-    <mergeCell ref="G6:G12"/>
     <mergeCell ref="D33:I33"/>
     <mergeCell ref="J33:P33"/>
     <mergeCell ref="D30:I30"/>
@@ -2012,6 +2050,13 @@
     <mergeCell ref="J31:P31"/>
     <mergeCell ref="D32:I32"/>
     <mergeCell ref="J32:P32"/>
+    <mergeCell ref="H6:H12"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="C6:C12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="F6:F12"/>
+    <mergeCell ref="G6:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2023,7 +2068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:C12"/>
     </sheetView>
   </sheetViews>
@@ -2035,11 +2080,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -2070,76 +2115,88 @@
     </row>
     <row r="6" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="71"/>
+      <c r="C6" s="88" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="67"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="71"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="67"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="87">
+        <f>('Période 1'!B8)+21</f>
+        <v>45803</v>
+      </c>
+      <c r="C8" s="62"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="67"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="71"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="67"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="71"/>
+      <c r="B10" s="87">
+        <f>('Période 1'!B10)+21</f>
+        <v>45821</v>
+      </c>
+      <c r="C10" s="62"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="67"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="71"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="67"/>
     </row>
     <row r="12" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="71"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2172,11 +2229,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -2207,76 +2264,76 @@
     </row>
     <row r="6" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="71"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="57"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="71"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="57"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="71"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="57"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="71"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="71"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="71"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="57"/>
     </row>
     <row r="12" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="71"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2309,12 +2366,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -2345,76 +2402,76 @@
     </row>
     <row r="6" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="71"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="57"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="71"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="57"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="71"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="57"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="71"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="71"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="71"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="57"/>
     </row>
     <row r="12" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="71"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2448,12 +2505,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -2484,76 +2541,76 @@
     </row>
     <row r="6" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="71"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="57"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="71"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="57"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="71"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="57"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="71"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="71"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="71"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="57"/>
     </row>
     <row r="12" spans="2:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="71"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>